<commit_message>
Added more meals and variety.
</commit_message>
<xml_diff>
--- a/Documentation/Benchmarks.xlsx
+++ b/Documentation/Benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\Antarctic-Food-Optimisation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C76AF7-28EA-4E9D-9C8B-4DAB936F1E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D529510-BDF7-4415-865C-58A725F2048C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2124" yWindow="2124" windowWidth="17280" windowHeight="8964" xr2:uid="{472969AF-E492-4476-AC40-D4572065F633}"/>
   </bookViews>
@@ -481,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{640751DF-F8E9-40E7-8456-464868000FDC}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28:F34"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Read in the master pax sheet and calculated physical intensity of roles.
</commit_message>
<xml_diff>
--- a/Documentation/Benchmarks.xlsx
+++ b/Documentation/Benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\Antarctic-Food-Optimisation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6186C1-A7F8-491D-8CCA-ABABC5A37B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0422E22-98F9-49B3-BB56-1DED53FB07EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{472969AF-E492-4476-AC40-D4572065F633}"/>
   </bookViews>
@@ -327,335 +327,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$41</c:f>
+              <c:f>Sheet1!$A$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>cost</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$B$40:$J$40</c:f>
-              <c:strCache>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>None</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>vareity lack</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>cost</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>emissions</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>calories (proxy for food waste)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>varietylack * 100000 + emissions</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>varietylack * emissions</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>varietylack + emissions + cost + calories</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>varietylack * 1000000 + emissions + cost + calories * 100</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$41:$J$41</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>551676</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>563155</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>548191</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>546214</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>546005</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>546214</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>546214</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>548353</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>546101</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EF72-4F7A-9791-1B2330D1821F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="411288591"/>
-        <c:axId val="411285679"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="411288591"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="411285679"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="411285679"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="411288591"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$42</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>emissions</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -919,7 +595,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -975,7 +651,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$43</c:f>
+              <c:f>Sheet1!$A$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1243,7 +919,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1567,7 +1243,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1836,6 +1512,330 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="632327823"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$43</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>emissions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$40:$J$40</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>None</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>vareity lack</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>cost</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>emissions</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>calories (proxy for food waste)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>varietylack * 100000 + emissions</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>varietylack * emissions</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>varietylack + emissions + cost + calories</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>varietylack * 1000000 + emissions + cost + calories * 100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$43:$J$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>12668638</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13184610</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12651894</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12456526</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12512566</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12456526</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12456526</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12565198</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12636718</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B1B7-4321-9705-CD083E75FB68}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="666089535"/>
+        <c:axId val="666084959"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="666089535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="666084959"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="666084959"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="666089535"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4611,42 +4611,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>115248</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>59306</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>420048</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>76890</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E890F44-E89A-934B-2553-E36000AD41EC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
       <xdr:colOff>94129</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>85165</xdr:rowOff>
@@ -4674,7 +4638,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4710,7 +4674,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4746,7 +4710,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4771,6 +4735,42 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1ABD29BB-B439-7349-6A78-0CE6A7C88642}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>79514</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>72887</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>384314</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>33131</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41A02A31-65CF-FDF8-CED1-AE100038396B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5090,8 +5090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{640751DF-F8E9-40E7-8456-464868000FDC}">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G36" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q45" sqref="Q45"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6090,7 +6090,7 @@
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B41">
         <v>551676</v>
@@ -6128,7 +6128,7 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B42">
         <v>14346668</v>
@@ -6166,7 +6166,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B43">
         <v>12668638</v>
@@ -6355,7 +6355,7 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B49">
         <v>6</v>
@@ -6387,7 +6387,7 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B50">
         <v>6</v>
@@ -6419,7 +6419,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B51">
         <v>6</v>

</xml_diff>

<commit_message>
Tried using nutrition sum in objective.
</commit_message>
<xml_diff>
--- a/Documentation/Benchmarks.xlsx
+++ b/Documentation/Benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\Antarctic-Food-Optimisation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A05396F-58BA-4357-9AC0-6C77E8F7BF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136C61C5-0F29-459E-9F49-2872E6D5EE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{472969AF-E492-4476-AC40-D4572065F633}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="82">
   <si>
     <t>cals</t>
   </si>
@@ -245,6 +245,42 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>occupancy data 7 days</t>
+  </si>
+  <si>
+    <t>cost + emissions + cals</t>
+  </si>
+  <si>
+    <t>relaxed constraints</t>
+  </si>
+  <si>
+    <t>30 s</t>
+  </si>
+  <si>
+    <t>cost + emissions*10 + cals * 1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost + emissions + cals * 100 </t>
+  </si>
+  <si>
+    <t>cost*10 + emissions + cals*100</t>
+  </si>
+  <si>
+    <t>cost*10 + emissions + cals*1000</t>
+  </si>
+  <si>
+    <t>sum(nutritionServed)</t>
+  </si>
+  <si>
+    <t>cost + emissions + sum(nutrition)</t>
+  </si>
+  <si>
+    <t>scaled avg</t>
+  </si>
+  <si>
+    <t>13th Jun</t>
   </si>
 </sst>
 </file>
@@ -1899,6 +1935,870 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="666089535"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$146</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>emissions</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$Q$147:$Q$149</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>cost £</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>emissions kg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>food waste cals</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$147:$R$149</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1768</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-59DE-4503-8DD9-E070464E3F06}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="940253424"/>
+        <c:axId val="940247184"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="940253424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="940247184"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="940247184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="940253424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$146</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cals</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$S$147:$S$149</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>cost £</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>emissions kg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>food waste cals</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$T$147:$T$149</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1790</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1913</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6ABB-4A7A-AD0F-8CF38EC18737}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="935028960"/>
+        <c:axId val="935029376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="935028960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="935029376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="935029376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="935028960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$V$146</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$U$147:$U$149</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>cost £</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>emissions kg</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>food waste cals</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$V$147:$V$149</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1766</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1863</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>867</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-63E4-420D-8D02-C5F56B8452F2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="1067882848"/>
+        <c:axId val="1067881184"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1067882848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1067881184"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1067881184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1067882848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2154,6 +3054,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4637,6 +5657,1517 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -4851,6 +7382,114 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>46383</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>351183</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>112644</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72FF912F-C1E0-BE13-1EAE-4F8676246093}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>364436</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>159026</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>59636</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>119269</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B180E6F-799C-3DC8-8DDC-756416D1B56F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>19880</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>172278</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>324680</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>132522</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9B4FAB2-A087-359F-81AF-8A7EB92D5EBE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5151,10 +7790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{640751DF-F8E9-40E7-8456-464868000FDC}">
-  <dimension ref="A1:S130"/>
+  <dimension ref="A1:V149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B127" sqref="B127"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D132" sqref="D132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7401,7 +10040,7 @@
         <v>7</v>
       </c>
       <c r="B117" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
@@ -7492,7 +10131,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>19</v>
       </c>
@@ -7500,12 +10139,284 @@
         <v>69</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>20</v>
       </c>
       <c r="B130" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D131" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>73</v>
+      </c>
+      <c r="B132" t="s">
+        <v>70</v>
+      </c>
+      <c r="D132" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>25</v>
+      </c>
+      <c r="B133" t="s">
+        <v>71</v>
+      </c>
+      <c r="C133" t="s">
+        <v>27</v>
+      </c>
+      <c r="D133" t="s">
+        <v>0</v>
+      </c>
+      <c r="E133" t="s">
+        <v>26</v>
+      </c>
+      <c r="F133" t="s">
+        <v>75</v>
+      </c>
+      <c r="G133" t="s">
+        <v>74</v>
+      </c>
+      <c r="H133" t="s">
+        <v>76</v>
+      </c>
+      <c r="I133" t="s">
+        <v>77</v>
+      </c>
+      <c r="J133" t="s">
+        <v>78</v>
+      </c>
+      <c r="K133" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>50</v>
+      </c>
+      <c r="B134">
+        <v>1768</v>
+      </c>
+      <c r="C134">
+        <v>1768</v>
+      </c>
+      <c r="D134">
+        <v>1790</v>
+      </c>
+      <c r="E134">
+        <v>1766</v>
+      </c>
+      <c r="F134">
+        <v>1768</v>
+      </c>
+      <c r="G134">
+        <v>1806</v>
+      </c>
+      <c r="H134">
+        <v>1768</v>
+      </c>
+      <c r="I134">
+        <v>1773</v>
+      </c>
+      <c r="J134">
+        <v>1768</v>
+      </c>
+      <c r="K134">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>51</v>
+      </c>
+      <c r="B135">
+        <v>1837</v>
+      </c>
+      <c r="C135">
+        <v>1837</v>
+      </c>
+      <c r="D135">
+        <v>1913</v>
+      </c>
+      <c r="E135">
+        <v>1863</v>
+      </c>
+      <c r="F135">
+        <v>1837</v>
+      </c>
+      <c r="G135">
+        <v>1868</v>
+      </c>
+      <c r="H135">
+        <v>1837</v>
+      </c>
+      <c r="I135">
+        <v>1892</v>
+      </c>
+      <c r="J135">
+        <v>1868</v>
+      </c>
+      <c r="K135">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>52</v>
+      </c>
+      <c r="B136">
+        <v>88619</v>
+      </c>
+      <c r="C136">
+        <v>87575</v>
+      </c>
+      <c r="D136">
+        <v>69575</v>
+      </c>
+      <c r="E136">
+        <v>86759</v>
+      </c>
+      <c r="F136">
+        <v>88619</v>
+      </c>
+      <c r="G136">
+        <v>78036</v>
+      </c>
+      <c r="H136">
+        <v>88619</v>
+      </c>
+      <c r="I136">
+        <v>77737</v>
+      </c>
+      <c r="J136">
+        <v>87634</v>
+      </c>
+      <c r="K136">
+        <v>88486</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>80</v>
+      </c>
+      <c r="B137">
+        <f>AVERAGE(B136/47, B135, B134)</f>
+        <v>1830.1702127659573</v>
+      </c>
+      <c r="C137">
+        <f t="shared" ref="C137:K137" si="4">AVERAGE(C136/47, C135, C134)</f>
+        <v>1822.7659574468087</v>
+      </c>
+      <c r="D137">
+        <f t="shared" si="4"/>
+        <v>1727.7730496453903</v>
+      </c>
+      <c r="E137">
+        <f t="shared" si="4"/>
+        <v>1824.9787234042553</v>
+      </c>
+      <c r="F137">
+        <f t="shared" si="4"/>
+        <v>1830.1702127659573</v>
+      </c>
+      <c r="G137">
+        <f t="shared" si="4"/>
+        <v>1778.113475177305</v>
+      </c>
+      <c r="H137">
+        <f t="shared" si="4"/>
+        <v>1830.1702127659573</v>
+      </c>
+      <c r="I137">
+        <f t="shared" si="4"/>
+        <v>1772.9929078014184</v>
+      </c>
+      <c r="J137">
+        <f t="shared" si="4"/>
+        <v>1833.5177304964539</v>
+      </c>
+      <c r="K137">
+        <f t="shared" si="4"/>
+        <v>1831.2269503546097</v>
+      </c>
+    </row>
+    <row r="146" spans="17:22" x14ac:dyDescent="0.3">
+      <c r="R146" t="s">
+        <v>27</v>
+      </c>
+      <c r="T146" t="s">
+        <v>0</v>
+      </c>
+      <c r="V146" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="147" spans="17:22" x14ac:dyDescent="0.3">
+      <c r="Q147" t="s">
+        <v>50</v>
+      </c>
+      <c r="R147">
+        <v>1768</v>
+      </c>
+      <c r="S147" t="s">
+        <v>50</v>
+      </c>
+      <c r="T147">
+        <v>1790</v>
+      </c>
+      <c r="U147" t="s">
+        <v>50</v>
+      </c>
+      <c r="V147">
+        <v>1766</v>
+      </c>
+    </row>
+    <row r="148" spans="17:22" x14ac:dyDescent="0.3">
+      <c r="Q148" t="s">
+        <v>51</v>
+      </c>
+      <c r="R148">
+        <v>1837</v>
+      </c>
+      <c r="S148" t="s">
+        <v>51</v>
+      </c>
+      <c r="T148">
+        <v>1913</v>
+      </c>
+      <c r="U148" t="s">
+        <v>51</v>
+      </c>
+      <c r="V148">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="149" spans="17:22" x14ac:dyDescent="0.3">
+      <c r="Q149" t="s">
+        <v>52</v>
+      </c>
+      <c r="R149">
+        <v>875</v>
+      </c>
+      <c r="S149" t="s">
+        <v>52</v>
+      </c>
+      <c r="T149">
+        <v>695</v>
+      </c>
+      <c r="U149" t="s">
+        <v>52</v>
+      </c>
+      <c r="V149">
+        <v>867</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Don't serve fresh food in winter.
</commit_message>
<xml_diff>
--- a/Documentation/Benchmarks.xlsx
+++ b/Documentation/Benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\Antarctic-Food-Optimisation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF5ACFE-A48B-4B4D-9C7F-E66D79C1D33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3839F6D-9B7A-44DB-8EA9-7D78533E627E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{472969AF-E492-4476-AC40-D4572065F633}"/>
+    <workbookView xWindow="5760" yWindow="3276" windowWidth="17280" windowHeight="8964" xr2:uid="{472969AF-E492-4476-AC40-D4572065F633}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="104">
   <si>
     <t>cals</t>
   </si>
@@ -282,6 +282,72 @@
   <si>
     <t>13th Jun</t>
   </si>
+  <si>
+    <t>15th Jun</t>
+  </si>
+  <si>
+    <t>Batch size</t>
+  </si>
+  <si>
+    <t>10 min</t>
+  </si>
+  <si>
+    <t>food waste sum nutrients</t>
+  </si>
+  <si>
+    <t>max num people</t>
+  </si>
+  <si>
+    <t>days x people</t>
+  </si>
+  <si>
+    <t>imporved over time</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>cost/(days x people)</t>
+  </si>
+  <si>
+    <t>emissions /(days x people)</t>
+  </si>
+  <si>
+    <t>food waste /(days x people)</t>
+  </si>
+  <si>
+    <t>satisfiability time</t>
+  </si>
+  <si>
+    <t>12 s</t>
+  </si>
+  <si>
+    <t>6 s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 s </t>
+  </si>
+  <si>
+    <t>1 m 15 s</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>1m</t>
+  </si>
+  <si>
+    <t>18 s</t>
+  </si>
+  <si>
+    <t>20 s</t>
+  </si>
+  <si>
+    <t>3m 56s</t>
+  </si>
+  <si>
+    <t>27s</t>
+  </si>
 </sst>
 </file>
 
@@ -340,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -348,6 +414,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7790,10 +7862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{640751DF-F8E9-40E7-8456-464868000FDC}">
-  <dimension ref="A1:V149"/>
+  <dimension ref="A1:V151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L144" sqref="L144"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D149" sqref="D149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10131,7 +10203,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>19</v>
       </c>
@@ -10139,7 +10211,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>20</v>
       </c>
@@ -10147,12 +10219,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D131" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>73</v>
       </c>
@@ -10163,7 +10235,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>25</v>
       </c>
@@ -10198,7 +10270,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>50</v>
       </c>
@@ -10233,7 +10305,7 @@
         <v>1771</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>51</v>
       </c>
@@ -10268,7 +10340,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>52</v>
       </c>
@@ -10303,7 +10375,7 @@
         <v>88486</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>80</v>
       </c>
@@ -10348,7 +10420,298 @@
         <v>1831.2269503546097</v>
       </c>
     </row>
-    <row r="146" spans="17:22" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>25</v>
+      </c>
+      <c r="B140" t="s">
+        <v>82</v>
+      </c>
+      <c r="C140" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>83</v>
+      </c>
+      <c r="B141" s="7">
+        <v>7</v>
+      </c>
+      <c r="C141" s="7">
+        <v>8</v>
+      </c>
+      <c r="D141" s="7">
+        <v>9</v>
+      </c>
+      <c r="E141" s="7">
+        <v>10</v>
+      </c>
+      <c r="F141" s="7">
+        <v>12</v>
+      </c>
+      <c r="G141" s="7">
+        <v>15</v>
+      </c>
+      <c r="H141" s="7">
+        <v>21</v>
+      </c>
+      <c r="I141" s="8">
+        <v>25</v>
+      </c>
+      <c r="J141" s="8">
+        <v>28</v>
+      </c>
+      <c r="K141" s="7">
+        <v>30</v>
+      </c>
+      <c r="L141" s="7">
+        <v>35</v>
+      </c>
+      <c r="M141" s="7">
+        <v>40</v>
+      </c>
+      <c r="N141" s="7">
+        <v>42</v>
+      </c>
+      <c r="O141" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>86</v>
+      </c>
+      <c r="B142" s="7">
+        <v>30</v>
+      </c>
+      <c r="C142" s="7">
+        <v>32</v>
+      </c>
+      <c r="D142" s="7">
+        <v>46</v>
+      </c>
+      <c r="E142" s="7">
+        <v>59</v>
+      </c>
+      <c r="F142" s="7">
+        <v>93</v>
+      </c>
+      <c r="G142" s="7">
+        <v>125</v>
+      </c>
+      <c r="H142" s="7">
+        <v>154</v>
+      </c>
+      <c r="I142" s="8">
+        <v>165</v>
+      </c>
+      <c r="J142" s="8">
+        <v>167</v>
+      </c>
+      <c r="K142" s="7">
+        <v>163</v>
+      </c>
+      <c r="L142" s="7">
+        <v>89</v>
+      </c>
+      <c r="M142" s="7">
+        <v>91</v>
+      </c>
+      <c r="N142" s="7">
+        <v>25</v>
+      </c>
+      <c r="O142" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>87</v>
+      </c>
+      <c r="B143" s="7">
+        <v>210</v>
+      </c>
+      <c r="C143" s="7">
+        <v>256</v>
+      </c>
+      <c r="D143" s="7">
+        <v>414</v>
+      </c>
+      <c r="E143" s="7">
+        <v>590</v>
+      </c>
+      <c r="F143" s="7">
+        <v>1116</v>
+      </c>
+      <c r="G143" s="7">
+        <v>1875</v>
+      </c>
+      <c r="H143" s="7">
+        <v>3234</v>
+      </c>
+      <c r="I143" s="8">
+        <v>4125</v>
+      </c>
+      <c r="J143" s="8">
+        <v>4676</v>
+      </c>
+      <c r="K143" s="7">
+        <v>4890</v>
+      </c>
+      <c r="L143" s="7">
+        <v>3115</v>
+      </c>
+      <c r="M143" s="7">
+        <v>3640</v>
+      </c>
+      <c r="N143" s="7">
+        <v>1050</v>
+      </c>
+      <c r="O143" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>93</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C144" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D144" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E144" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F144" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="G144" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H144" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I144" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="J144" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="K144" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="L144" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="M144" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N144" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="O144" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="145" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>88</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D145" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E145" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F145" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="G145" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H145" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I145" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="J145" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="K145" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="L145" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="M145" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N145" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="O145" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="146" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>50</v>
+      </c>
+      <c r="B146" s="8">
+        <v>1713</v>
+      </c>
+      <c r="C146" s="8">
+        <v>1966</v>
+      </c>
+      <c r="D146" s="8">
+        <v>3149</v>
+      </c>
+      <c r="E146" s="8">
+        <v>3677</v>
+      </c>
+      <c r="F146">
+        <v>6497</v>
+      </c>
+      <c r="G146">
+        <v>13222</v>
+      </c>
+      <c r="H146">
+        <v>23956</v>
+      </c>
+      <c r="I146">
+        <v>35142</v>
+      </c>
+      <c r="J146">
+        <v>39977</v>
+      </c>
+      <c r="K146">
+        <v>33533</v>
+      </c>
+      <c r="L146">
+        <v>26349</v>
+      </c>
+      <c r="M146" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N146">
+        <v>8953</v>
+      </c>
+      <c r="O146" t="s">
+        <v>50</v>
+      </c>
       <c r="R146" t="s">
         <v>27</v>
       </c>
@@ -10359,7 +10722,52 @@
         <v>26</v>
       </c>
     </row>
-    <row r="147" spans="17:22" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>51</v>
+      </c>
+      <c r="B147" s="8">
+        <v>1632</v>
+      </c>
+      <c r="C147" s="8">
+        <v>2031</v>
+      </c>
+      <c r="D147" s="8">
+        <v>3068</v>
+      </c>
+      <c r="E147" s="8">
+        <v>3322</v>
+      </c>
+      <c r="F147">
+        <v>6027</v>
+      </c>
+      <c r="G147">
+        <v>11915</v>
+      </c>
+      <c r="H147">
+        <v>22637</v>
+      </c>
+      <c r="I147">
+        <v>32098</v>
+      </c>
+      <c r="J147">
+        <v>35670</v>
+      </c>
+      <c r="K147">
+        <v>34496</v>
+      </c>
+      <c r="L147">
+        <v>25271</v>
+      </c>
+      <c r="M147" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N147">
+        <v>9003</v>
+      </c>
+      <c r="O147" t="s">
+        <v>51</v>
+      </c>
       <c r="Q147" t="s">
         <v>50</v>
       </c>
@@ -10379,7 +10787,52 @@
         <v>1766</v>
       </c>
     </row>
-    <row r="148" spans="17:22" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>85</v>
+      </c>
+      <c r="B148" s="8">
+        <v>74168</v>
+      </c>
+      <c r="C148" s="8">
+        <v>74014</v>
+      </c>
+      <c r="D148" s="8">
+        <v>136986</v>
+      </c>
+      <c r="E148" s="8">
+        <v>148030</v>
+      </c>
+      <c r="F148">
+        <v>337583</v>
+      </c>
+      <c r="G148">
+        <v>388942</v>
+      </c>
+      <c r="H148">
+        <v>752213</v>
+      </c>
+      <c r="I148">
+        <v>1107399</v>
+      </c>
+      <c r="J148">
+        <v>922383</v>
+      </c>
+      <c r="K148">
+        <v>1892849</v>
+      </c>
+      <c r="L148">
+        <v>1129074</v>
+      </c>
+      <c r="M148" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N148">
+        <v>445200</v>
+      </c>
+      <c r="O148" t="s">
+        <v>85</v>
+      </c>
       <c r="Q148" t="s">
         <v>51</v>
       </c>
@@ -10399,7 +10852,64 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="149" spans="17:22" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>90</v>
+      </c>
+      <c r="B149" s="8">
+        <f>1713/210</f>
+        <v>8.1571428571428566</v>
+      </c>
+      <c r="C149" s="8">
+        <f>1966/256</f>
+        <v>7.6796875</v>
+      </c>
+      <c r="D149" s="8">
+        <f>3149/414</f>
+        <v>7.6062801932367146</v>
+      </c>
+      <c r="E149" s="8">
+        <f>3677/590</f>
+        <v>6.2322033898305085</v>
+      </c>
+      <c r="F149">
+        <f>6497/1116</f>
+        <v>5.8216845878136203</v>
+      </c>
+      <c r="G149">
+        <f>13222/1875</f>
+        <v>7.051733333333333</v>
+      </c>
+      <c r="H149">
+        <f>23956/3234</f>
+        <v>7.4075448361162648</v>
+      </c>
+      <c r="I149">
+        <f>35142/4125</f>
+        <v>8.5192727272727264</v>
+      </c>
+      <c r="J149">
+        <f>39977/4676</f>
+        <v>8.5494011976047908</v>
+      </c>
+      <c r="K149">
+        <f>33533/4890</f>
+        <v>6.8574642126789369</v>
+      </c>
+      <c r="L149">
+        <f>26349/3115</f>
+        <v>8.4587479935794541</v>
+      </c>
+      <c r="M149" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N149">
+        <f>8953/1050</f>
+        <v>8.5266666666666673</v>
+      </c>
+      <c r="O149" t="s">
+        <v>90</v>
+      </c>
       <c r="Q149" t="s">
         <v>52</v>
       </c>
@@ -10417,6 +10927,124 @@
       </c>
       <c r="V149">
         <v>867</v>
+      </c>
+    </row>
+    <row r="150" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>91</v>
+      </c>
+      <c r="B150" s="8">
+        <f>1632/210</f>
+        <v>7.7714285714285714</v>
+      </c>
+      <c r="C150" s="8">
+        <f>2031/256</f>
+        <v>7.93359375</v>
+      </c>
+      <c r="D150" s="8">
+        <f>3068/414</f>
+        <v>7.4106280193236715</v>
+      </c>
+      <c r="E150" s="8">
+        <f>3322/590</f>
+        <v>5.6305084745762715</v>
+      </c>
+      <c r="F150">
+        <f>6027/1116</f>
+        <v>5.400537634408602</v>
+      </c>
+      <c r="G150">
+        <f>11915/1875</f>
+        <v>6.3546666666666667</v>
+      </c>
+      <c r="H150">
+        <f>22637/3234</f>
+        <v>6.9996907854050709</v>
+      </c>
+      <c r="I150">
+        <f>32098/4125</f>
+        <v>7.7813333333333334</v>
+      </c>
+      <c r="J150">
+        <f>35670/4676</f>
+        <v>7.6283147989734816</v>
+      </c>
+      <c r="K150">
+        <f>34496/4890</f>
+        <v>7.0543967280163598</v>
+      </c>
+      <c r="L150">
+        <f>25271/3115</f>
+        <v>8.1126805778491171</v>
+      </c>
+      <c r="M150" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N150">
+        <f>9003/1050</f>
+        <v>8.5742857142857147</v>
+      </c>
+      <c r="O150" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="151" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>92</v>
+      </c>
+      <c r="B151" s="8">
+        <f>74168/210</f>
+        <v>353.18095238095236</v>
+      </c>
+      <c r="C151" s="8">
+        <f>74014/256</f>
+        <v>289.1171875</v>
+      </c>
+      <c r="D151" s="8">
+        <f>136986/414</f>
+        <v>330.8840579710145</v>
+      </c>
+      <c r="E151" s="8">
+        <f>148030/590</f>
+        <v>250.89830508474577</v>
+      </c>
+      <c r="F151">
+        <f>337583/1116</f>
+        <v>302.4937275985663</v>
+      </c>
+      <c r="G151">
+        <f>388942/1875</f>
+        <v>207.43573333333333</v>
+      </c>
+      <c r="H151">
+        <f>752213/3234</f>
+        <v>232.5952380952381</v>
+      </c>
+      <c r="I151">
+        <f>1107399/4125</f>
+        <v>268.46036363636364</v>
+      </c>
+      <c r="J151">
+        <f>922383/4676</f>
+        <v>197.25898203592814</v>
+      </c>
+      <c r="K151">
+        <f>1892849/4890</f>
+        <v>387.08568507157463</v>
+      </c>
+      <c r="L151">
+        <f>1129074/3115</f>
+        <v>362.46356340288924</v>
+      </c>
+      <c r="M151" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="N151">
+        <f>445200/1050</f>
+        <v>424</v>
+      </c>
+      <c r="O151" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Split data into batches according to max matrix size.
</commit_message>
<xml_diff>
--- a/Documentation/Benchmarks.xlsx
+++ b/Documentation/Benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\Antarctic-Food-Optimisation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3839F6D-9B7A-44DB-8EA9-7D78533E627E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E309680-10B3-4F83-8692-EC41606F7C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="3276" windowWidth="17280" windowHeight="8964" xr2:uid="{472969AF-E492-4476-AC40-D4572065F633}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="109">
   <si>
     <t>cals</t>
   </si>
@@ -347,6 +347,21 @@
   </si>
   <si>
     <t>27s</t>
+  </si>
+  <si>
+    <t>16th Jun</t>
+  </si>
+  <si>
+    <t>5 min</t>
+  </si>
+  <si>
+    <t>Matrix size</t>
+  </si>
+  <si>
+    <t>test runs</t>
+  </si>
+  <si>
+    <t>actual run</t>
   </si>
 </sst>
 </file>
@@ -7862,10 +7877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{640751DF-F8E9-40E7-8456-464868000FDC}">
-  <dimension ref="A1:V151"/>
+  <dimension ref="A1:V170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D149" sqref="D149"/>
+    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F164" sqref="F164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11047,6 +11062,398 @@
         <v>92</v>
       </c>
     </row>
+    <row r="154" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>25</v>
+      </c>
+      <c r="B154" t="s">
+        <v>104</v>
+      </c>
+      <c r="C154" t="s">
+        <v>105</v>
+      </c>
+      <c r="D154" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="155" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>106</v>
+      </c>
+      <c r="B155">
+        <v>104</v>
+      </c>
+      <c r="C155">
+        <v>204</v>
+      </c>
+      <c r="D155">
+        <v>511</v>
+      </c>
+      <c r="E155">
+        <v>1037</v>
+      </c>
+      <c r="F155">
+        <v>1568</v>
+      </c>
+      <c r="G155">
+        <v>2149</v>
+      </c>
+      <c r="H155">
+        <v>2657</v>
+      </c>
+      <c r="I155">
+        <v>3075</v>
+      </c>
+      <c r="J155">
+        <v>3505</v>
+      </c>
+      <c r="K155">
+        <v>4025</v>
+      </c>
+      <c r="L155">
+        <v>5043</v>
+      </c>
+      <c r="M155">
+        <v>6085</v>
+      </c>
+    </row>
+    <row r="156" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>50</v>
+      </c>
+      <c r="B156">
+        <v>851</v>
+      </c>
+      <c r="C156">
+        <v>1821</v>
+      </c>
+      <c r="D156">
+        <v>4617</v>
+      </c>
+      <c r="E156">
+        <v>9044</v>
+      </c>
+      <c r="F156">
+        <v>14108</v>
+      </c>
+      <c r="G156">
+        <v>18991</v>
+      </c>
+      <c r="H156">
+        <v>23556</v>
+      </c>
+      <c r="I156">
+        <v>27895</v>
+      </c>
+      <c r="J156">
+        <v>31368</v>
+      </c>
+      <c r="K156" t="s">
+        <v>45</v>
+      </c>
+      <c r="L156" t="s">
+        <v>45</v>
+      </c>
+      <c r="M156" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="157" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>51</v>
+      </c>
+      <c r="B157">
+        <v>865</v>
+      </c>
+      <c r="C157">
+        <v>1646</v>
+      </c>
+      <c r="D157">
+        <v>4454</v>
+      </c>
+      <c r="E157">
+        <v>8634</v>
+      </c>
+      <c r="F157">
+        <v>12212</v>
+      </c>
+      <c r="G157">
+        <v>17782</v>
+      </c>
+      <c r="H157">
+        <v>21449</v>
+      </c>
+      <c r="I157">
+        <v>25804</v>
+      </c>
+      <c r="J157">
+        <v>28934</v>
+      </c>
+      <c r="K157" t="s">
+        <v>45</v>
+      </c>
+      <c r="L157" t="s">
+        <v>45</v>
+      </c>
+      <c r="M157" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="158" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>85</v>
+      </c>
+      <c r="B158">
+        <v>58649</v>
+      </c>
+      <c r="C158">
+        <v>79523</v>
+      </c>
+      <c r="D158">
+        <v>182057</v>
+      </c>
+      <c r="E158">
+        <v>401520</v>
+      </c>
+      <c r="F158">
+        <v>617231</v>
+      </c>
+      <c r="G158">
+        <v>763670</v>
+      </c>
+      <c r="H158">
+        <v>1104941</v>
+      </c>
+      <c r="I158">
+        <v>1039116</v>
+      </c>
+      <c r="J158">
+        <v>1490343</v>
+      </c>
+      <c r="K158" t="s">
+        <v>45</v>
+      </c>
+      <c r="L158" t="s">
+        <v>45</v>
+      </c>
+      <c r="M158" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="159" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>90</v>
+      </c>
+      <c r="B159">
+        <f>851/104</f>
+        <v>8.1826923076923084</v>
+      </c>
+      <c r="C159">
+        <f>1821/204</f>
+        <v>8.9264705882352935</v>
+      </c>
+      <c r="D159">
+        <f>4617/511</f>
+        <v>9.0352250489236798</v>
+      </c>
+      <c r="E159">
+        <f>9044/1037</f>
+        <v>8.721311475409836</v>
+      </c>
+      <c r="F159">
+        <f>14108/1568</f>
+        <v>8.9974489795918373</v>
+      </c>
+      <c r="G159">
+        <f>18991/2149</f>
+        <v>8.8371335504886002</v>
+      </c>
+      <c r="H159">
+        <f>23556/2657</f>
+        <v>8.8656379375235232</v>
+      </c>
+      <c r="I159">
+        <f>27895/3075</f>
+        <v>9.0715447154471551</v>
+      </c>
+      <c r="J159">
+        <f>31368/3505</f>
+        <v>8.9495007132667617</v>
+      </c>
+      <c r="K159" t="s">
+        <v>45</v>
+      </c>
+      <c r="L159" t="s">
+        <v>45</v>
+      </c>
+      <c r="M159" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="160" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>91</v>
+      </c>
+      <c r="B160">
+        <f>865/104</f>
+        <v>8.3173076923076916</v>
+      </c>
+      <c r="C160">
+        <f>1646/204</f>
+        <v>8.0686274509803919</v>
+      </c>
+      <c r="D160">
+        <f>4454/511</f>
+        <v>8.7162426614481401</v>
+      </c>
+      <c r="E160">
+        <f>8634/1037</f>
+        <v>8.3259402121504333</v>
+      </c>
+      <c r="F160">
+        <f>12212/1568</f>
+        <v>7.7882653061224492</v>
+      </c>
+      <c r="G160">
+        <f>17782/2149</f>
+        <v>8.274546300604932</v>
+      </c>
+      <c r="H160">
+        <f>21449/2657</f>
+        <v>8.0726383138878433</v>
+      </c>
+      <c r="I160">
+        <f>25804/3075</f>
+        <v>8.3915447154471536</v>
+      </c>
+      <c r="J160">
+        <f>28934/3505</f>
+        <v>8.2550641940085594</v>
+      </c>
+      <c r="K160" t="s">
+        <v>45</v>
+      </c>
+      <c r="L160" t="s">
+        <v>45</v>
+      </c>
+      <c r="M160" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>92</v>
+      </c>
+      <c r="B161">
+        <f>58649/104</f>
+        <v>563.93269230769226</v>
+      </c>
+      <c r="C161">
+        <f>79523/204</f>
+        <v>389.81862745098039</v>
+      </c>
+      <c r="D161">
+        <f>182057/511</f>
+        <v>356.27592954990217</v>
+      </c>
+      <c r="E161">
+        <f>401520/1037</f>
+        <v>387.19382835101254</v>
+      </c>
+      <c r="F161">
+        <f>617231/1568</f>
+        <v>393.64221938775512</v>
+      </c>
+      <c r="G161">
+        <f>763670/2149</f>
+        <v>355.36063285248952</v>
+      </c>
+      <c r="H161">
+        <f>1104941/2657</f>
+        <v>415.86036883703423</v>
+      </c>
+      <c r="I161">
+        <f>1039116/3075</f>
+        <v>337.9239024390244</v>
+      </c>
+      <c r="J161">
+        <f>1490343/3505</f>
+        <v>425.20485021398002</v>
+      </c>
+      <c r="K161" t="s">
+        <v>45</v>
+      </c>
+      <c r="L161" t="s">
+        <v>45</v>
+      </c>
+      <c r="M161" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>106</v>
+      </c>
+      <c r="B164">
+        <v>3505</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>50</v>
+      </c>
+      <c r="B165">
+        <v>25848</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
+        <v>51</v>
+      </c>
+      <c r="B166">
+        <v>22713</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
+        <v>85</v>
+      </c>
+      <c r="B167">
+        <v>776138</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>90</v>
+      </c>
+      <c r="B168">
+        <f>25848/3505</f>
+        <v>7.3746077032810273</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
+        <v>91</v>
+      </c>
+      <c r="B169">
+        <f>22713/3505</f>
+        <v>6.4801711840228249</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
+        <v>92</v>
+      </c>
+      <c r="B170">
+        <f>776138/3505</f>
+        <v>221.4373751783167</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Merged loops in places where it helped reduce the solving time.
</commit_message>
<xml_diff>
--- a/Documentation/Benchmarks.xlsx
+++ b/Documentation/Benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\Antarctic-Food-Optimisation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E309680-10B3-4F83-8692-EC41606F7C7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7B9BD9-0D9D-4391-92C7-4ABEE7E7137B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3276" windowWidth="17280" windowHeight="8964" xr2:uid="{472969AF-E492-4476-AC40-D4572065F633}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{472969AF-E492-4476-AC40-D4572065F633}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -7880,7 +7880,7 @@
   <dimension ref="A1:V170"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A153" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F164" sqref="F164"/>
+      <selection activeCell="C165" sqref="C165:C167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Generated output for all data.
</commit_message>
<xml_diff>
--- a/Documentation/Benchmarks.xlsx
+++ b/Documentation/Benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\Antarctic-Food-Optimisation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7B9BD9-0D9D-4391-92C7-4ABEE7E7137B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247630EE-6275-4999-A277-0800DC5A4206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{472969AF-E492-4476-AC40-D4572065F633}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="111">
   <si>
     <t>cals</t>
   </si>
@@ -361,7 +361,13 @@
     <t>test runs</t>
   </si>
   <si>
-    <t>actual run</t>
+    <t>actual batch</t>
+  </si>
+  <si>
+    <t>no beef or lamb</t>
+  </si>
+  <si>
+    <t>batch</t>
   </si>
 </sst>
 </file>
@@ -7877,15 +7883,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{640751DF-F8E9-40E7-8456-464868000FDC}">
-  <dimension ref="A1:V170"/>
+  <dimension ref="A1:V180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C165" sqref="C165:C167"/>
+    <sheetView tabSelected="1" topLeftCell="A162" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I178" sqref="I178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="3" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11394,13 +11400,64 @@
       <c r="A163" t="s">
         <v>108</v>
       </c>
+      <c r="B163">
+        <v>1</v>
+      </c>
+      <c r="C163">
+        <v>2</v>
+      </c>
+      <c r="D163">
+        <v>3</v>
+      </c>
+      <c r="E163">
+        <v>4</v>
+      </c>
+      <c r="F163">
+        <v>5</v>
+      </c>
+      <c r="G163">
+        <v>6</v>
+      </c>
+      <c r="H163">
+        <v>7</v>
+      </c>
+      <c r="I163">
+        <v>8</v>
+      </c>
+      <c r="J163">
+        <v>9</v>
+      </c>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>106</v>
       </c>
       <c r="B164">
-        <v>3505</v>
+        <v>3011</v>
+      </c>
+      <c r="C164">
+        <v>3149</v>
+      </c>
+      <c r="D164">
+        <v>3054</v>
+      </c>
+      <c r="E164">
+        <v>3093</v>
+      </c>
+      <c r="F164">
+        <v>3154</v>
+      </c>
+      <c r="G164">
+        <v>3077</v>
+      </c>
+      <c r="H164">
+        <v>3026</v>
+      </c>
+      <c r="I164">
+        <v>3012</v>
+      </c>
+      <c r="J164">
+        <v>2000</v>
       </c>
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.3">
@@ -11408,7 +11465,31 @@
         <v>50</v>
       </c>
       <c r="B165">
-        <v>25848</v>
+        <v>27241</v>
+      </c>
+      <c r="C165">
+        <v>30681</v>
+      </c>
+      <c r="D165">
+        <v>31253</v>
+      </c>
+      <c r="E165">
+        <v>29389</v>
+      </c>
+      <c r="F165">
+        <v>30123</v>
+      </c>
+      <c r="G165">
+        <v>30477</v>
+      </c>
+      <c r="H165">
+        <v>29196</v>
+      </c>
+      <c r="I165">
+        <v>28656</v>
+      </c>
+      <c r="J165">
+        <v>20250</v>
       </c>
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.3">
@@ -11416,7 +11497,31 @@
         <v>51</v>
       </c>
       <c r="B166">
-        <v>22713</v>
+        <v>24796</v>
+      </c>
+      <c r="C166">
+        <v>27340</v>
+      </c>
+      <c r="D166">
+        <v>27585</v>
+      </c>
+      <c r="E166">
+        <v>28174</v>
+      </c>
+      <c r="F166">
+        <v>28021</v>
+      </c>
+      <c r="G166">
+        <v>27233</v>
+      </c>
+      <c r="H166">
+        <v>25906</v>
+      </c>
+      <c r="I166">
+        <v>24330</v>
+      </c>
+      <c r="J166">
+        <v>17068</v>
       </c>
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.3">
@@ -11424,7 +11529,31 @@
         <v>85</v>
       </c>
       <c r="B167">
-        <v>776138</v>
+        <v>1128873</v>
+      </c>
+      <c r="C167">
+        <v>826028</v>
+      </c>
+      <c r="D167">
+        <v>747515</v>
+      </c>
+      <c r="E167">
+        <v>1252003</v>
+      </c>
+      <c r="F167">
+        <v>1043889</v>
+      </c>
+      <c r="G167">
+        <v>852864</v>
+      </c>
+      <c r="H167">
+        <v>768373</v>
+      </c>
+      <c r="I167">
+        <v>1098457</v>
+      </c>
+      <c r="J167">
+        <v>607663</v>
       </c>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.3">
@@ -11432,8 +11561,40 @@
         <v>90</v>
       </c>
       <c r="B168">
-        <f>25848/3505</f>
-        <v>7.3746077032810273</v>
+        <f>(27241/3011)</f>
+        <v>9.0471604118233149</v>
+      </c>
+      <c r="C168">
+        <f>30681/3149</f>
+        <v>9.743093045411241</v>
+      </c>
+      <c r="D168">
+        <f>31253/3054</f>
+        <v>10.233464309102816</v>
+      </c>
+      <c r="E168">
+        <f>29389/3093</f>
+        <v>9.5017782088587133</v>
+      </c>
+      <c r="F168">
+        <f>30123/3154</f>
+        <v>9.5507292327203555</v>
+      </c>
+      <c r="G168">
+        <f>30477/3077</f>
+        <v>9.904777380565486</v>
+      </c>
+      <c r="H168">
+        <f>29196/3026</f>
+        <v>9.6483807005948439</v>
+      </c>
+      <c r="I168">
+        <f>28656/3012</f>
+        <v>9.5139442231075702</v>
+      </c>
+      <c r="J168">
+        <f>20250/2000</f>
+        <v>10.125</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.3">
@@ -11441,8 +11602,40 @@
         <v>91</v>
       </c>
       <c r="B169">
-        <f>22713/3505</f>
-        <v>6.4801711840228249</v>
+        <f>(24796/3011)</f>
+        <v>8.235137827964131</v>
+      </c>
+      <c r="C169">
+        <f>27340/3149</f>
+        <v>8.6821213083518582</v>
+      </c>
+      <c r="D169">
+        <f>27585/3054</f>
+        <v>9.0324165029469548</v>
+      </c>
+      <c r="E169">
+        <f>28174/3093</f>
+        <v>9.1089557064338837</v>
+      </c>
+      <c r="F169">
+        <f>28021/3154</f>
+        <v>8.8842739378566904</v>
+      </c>
+      <c r="G169">
+        <f>27233/3077</f>
+        <v>8.850503737406564</v>
+      </c>
+      <c r="H169">
+        <f>25906/3026</f>
+        <v>8.5611368142762725</v>
+      </c>
+      <c r="I169">
+        <f>24330/3012</f>
+        <v>8.0776892430278888</v>
+      </c>
+      <c r="J169">
+        <f>17068/2000</f>
+        <v>8.5340000000000007</v>
       </c>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.3">
@@ -11450,8 +11643,139 @@
         <v>92</v>
       </c>
       <c r="B170">
-        <f>776138/3505</f>
-        <v>221.4373751783167</v>
+        <f>(1128873/3011)</f>
+        <v>374.91630687479244</v>
+      </c>
+      <c r="C170">
+        <f>826028/3149</f>
+        <v>262.31438551921246</v>
+      </c>
+      <c r="D170">
+        <f>747515/3054</f>
+        <v>244.76588081204977</v>
+      </c>
+      <c r="E170">
+        <f>1252003/3093</f>
+        <v>404.78596831555126</v>
+      </c>
+      <c r="F170">
+        <f>1043889/3154</f>
+        <v>330.97305009511729</v>
+      </c>
+      <c r="G170">
+        <f>852864/3077</f>
+        <v>277.17387065323368</v>
+      </c>
+      <c r="H170">
+        <f>768373/3026</f>
+        <v>253.92366159947125</v>
+      </c>
+      <c r="I170">
+        <f>1098457/3012</f>
+        <v>364.69355909694553</v>
+      </c>
+      <c r="J170">
+        <f>607663/2000</f>
+        <v>303.83150000000001</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A172" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A173" t="s">
+        <v>110</v>
+      </c>
+      <c r="B173">
+        <v>1</v>
+      </c>
+      <c r="J173">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>106</v>
+      </c>
+      <c r="B174">
+        <v>3011</v>
+      </c>
+      <c r="J174">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A175" t="s">
+        <v>50</v>
+      </c>
+      <c r="B175">
+        <v>27665</v>
+      </c>
+      <c r="J175">
+        <v>20337</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A176" t="s">
+        <v>51</v>
+      </c>
+      <c r="B176">
+        <v>21977</v>
+      </c>
+      <c r="J176">
+        <v>15733</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A177" t="s">
+        <v>85</v>
+      </c>
+      <c r="B177">
+        <v>830515</v>
+      </c>
+      <c r="J177">
+        <v>600977</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A178" t="s">
+        <v>90</v>
+      </c>
+      <c r="B178">
+        <f>27665/3011</f>
+        <v>9.1879774161408179</v>
+      </c>
+      <c r="J178">
+        <f>20337/2000</f>
+        <v>10.1685</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A179" t="s">
+        <v>91</v>
+      </c>
+      <c r="B179">
+        <f>21977/3011</f>
+        <v>7.2989040185984724</v>
+      </c>
+      <c r="J179">
+        <f>15733/2000</f>
+        <v>7.8665000000000003</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>92</v>
+      </c>
+      <c r="B180">
+        <f>830515/3011</f>
+        <v>275.82696778478913</v>
+      </c>
+      <c r="J180">
+        <f>600977/2000</f>
+        <v>300.48849999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Output menu to spreadsheet.
</commit_message>
<xml_diff>
--- a/Documentation/Benchmarks.xlsx
+++ b/Documentation/Benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\Antarctic-Food-Optimisation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247630EE-6275-4999-A277-0800DC5A4206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C550C0-E5E0-4EF2-9F68-D5D266B4F764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{472969AF-E492-4476-AC40-D4572065F633}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="116">
   <si>
     <t>cals</t>
   </si>
@@ -368,6 +368,21 @@
   </si>
   <si>
     <t>batch</t>
+  </si>
+  <si>
+    <t>total for 370 days</t>
+  </si>
+  <si>
+    <t>winter</t>
+  </si>
+  <si>
+    <t>year average</t>
+  </si>
+  <si>
+    <t>winter average</t>
+  </si>
+  <si>
+    <t>summer average</t>
   </si>
 </sst>
 </file>
@@ -7885,14 +7900,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{640751DF-F8E9-40E7-8456-464868000FDC}">
   <dimension ref="A1:V180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I178" sqref="I178"/>
+    <sheetView tabSelected="1" topLeftCell="A165" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O190" sqref="O190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="3" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.77734375" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
@@ -11346,7 +11364,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>92</v>
       </c>
@@ -11396,7 +11414,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I162" t="s">
+        <v>112</v>
+      </c>
+      <c r="J162" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>108</v>
       </c>
@@ -11428,7 +11454,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>106</v>
       </c>
@@ -11459,8 +11485,11 @@
       <c r="J164">
         <v>2000</v>
       </c>
-    </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K164" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>50</v>
       </c>
@@ -11491,8 +11520,12 @@
       <c r="J165">
         <v>20250</v>
       </c>
-    </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K165">
+        <f>SUM(B165:J165)</f>
+        <v>257266</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>51</v>
       </c>
@@ -11523,8 +11556,12 @@
       <c r="J166">
         <v>17068</v>
       </c>
-    </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K166">
+        <f>SUM(B166:J166)</f>
+        <v>230453</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>85</v>
       </c>
@@ -11555,8 +11592,21 @@
       <c r="J167">
         <v>607663</v>
       </c>
-    </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K167">
+        <f>SUM(B167:J167)</f>
+        <v>8325665</v>
+      </c>
+      <c r="L167" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="M167" t="s">
+        <v>115</v>
+      </c>
+      <c r="N167" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>90</v>
       </c>
@@ -11596,8 +11646,20 @@
         <f>20250/2000</f>
         <v>10.125</v>
       </c>
-    </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L168">
+        <f>AVERAGE(B168:J168)</f>
+        <v>9.6964808346871489</v>
+      </c>
+      <c r="M168">
+        <f>AVERAGE(B168:H168)</f>
+        <v>9.6613404698681098</v>
+      </c>
+      <c r="N168">
+        <f>AVERAGE(I168:J168)</f>
+        <v>9.819472111553786</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>91</v>
       </c>
@@ -11637,8 +11699,20 @@
         <f>17068/2000</f>
         <v>8.5340000000000007</v>
       </c>
-    </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L169">
+        <f>AVERAGE(B169:J169)</f>
+        <v>8.6629150086960269</v>
+      </c>
+      <c r="M169">
+        <f t="shared" ref="M169:M170" si="5">AVERAGE(B169:H169)</f>
+        <v>8.76493511931948</v>
+      </c>
+      <c r="N169">
+        <f>AVERAGE(I169:J169)</f>
+        <v>8.3058446215139448</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>92</v>
       </c>
@@ -11678,68 +11752,206 @@
         <f>607663/2000</f>
         <v>303.83150000000001</v>
       </c>
-    </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L170">
+        <f>AVERAGE(B170:J170)</f>
+        <v>313.04202032959711</v>
+      </c>
+      <c r="M170">
+        <f t="shared" si="5"/>
+        <v>306.97901769563259</v>
+      </c>
+      <c r="N170">
+        <f>AVERAGE(I170:J170)</f>
+        <v>334.2625295484728</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I172" t="s">
+        <v>112</v>
+      </c>
+      <c r="J172" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>110</v>
       </c>
       <c r="B173">
         <v>1</v>
       </c>
+      <c r="C173">
+        <v>2</v>
+      </c>
+      <c r="D173">
+        <v>3</v>
+      </c>
+      <c r="E173">
+        <v>4</v>
+      </c>
+      <c r="F173">
+        <v>5</v>
+      </c>
+      <c r="G173">
+        <v>6</v>
+      </c>
+      <c r="H173">
+        <v>7</v>
+      </c>
+      <c r="I173">
+        <v>8</v>
+      </c>
       <c r="J173">
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>106</v>
       </c>
       <c r="B174">
         <v>3011</v>
       </c>
+      <c r="C174">
+        <v>3149</v>
+      </c>
+      <c r="D174">
+        <v>3054</v>
+      </c>
+      <c r="E174">
+        <v>3093</v>
+      </c>
+      <c r="F174">
+        <v>3154</v>
+      </c>
+      <c r="G174">
+        <v>3077</v>
+      </c>
+      <c r="H174">
+        <v>3026</v>
+      </c>
+      <c r="I174">
+        <v>3012</v>
+      </c>
       <c r="J174">
         <v>2000</v>
       </c>
-    </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K174" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>50</v>
       </c>
       <c r="B175">
         <v>27665</v>
       </c>
+      <c r="C175">
+        <v>28349</v>
+      </c>
+      <c r="D175">
+        <v>27874</v>
+      </c>
+      <c r="E175">
+        <v>30408</v>
+      </c>
+      <c r="F175">
+        <v>30552</v>
+      </c>
+      <c r="H175">
+        <v>27287</v>
+      </c>
+      <c r="I175">
+        <v>29005</v>
+      </c>
       <c r="J175">
         <v>20337</v>
       </c>
-    </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K175">
+        <f>SUM(B175:J175)</f>
+        <v>221477</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>51</v>
       </c>
       <c r="B176">
         <v>21977</v>
       </c>
+      <c r="C176">
+        <v>23656</v>
+      </c>
+      <c r="D176">
+        <v>24225</v>
+      </c>
+      <c r="E176">
+        <v>26364</v>
+      </c>
+      <c r="F176">
+        <v>26706</v>
+      </c>
+      <c r="H176">
+        <v>24405</v>
+      </c>
+      <c r="I176">
+        <v>22464</v>
+      </c>
       <c r="J176">
         <v>15733</v>
       </c>
-    </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K176">
+        <f t="shared" ref="K176:K177" si="6">SUM(B176:J176)</f>
+        <v>185530</v>
+      </c>
+    </row>
+    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>85</v>
       </c>
       <c r="B177">
         <v>830515</v>
       </c>
+      <c r="C177">
+        <v>836547</v>
+      </c>
+      <c r="D177">
+        <v>844315</v>
+      </c>
+      <c r="E177">
+        <v>800038</v>
+      </c>
+      <c r="F177">
+        <v>968130</v>
+      </c>
+      <c r="H177">
+        <v>1215430</v>
+      </c>
+      <c r="I177">
+        <v>1061965</v>
+      </c>
       <c r="J177">
         <v>600977</v>
       </c>
-    </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K177">
+        <f t="shared" si="6"/>
+        <v>7157917</v>
+      </c>
+      <c r="L177" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="M177" t="s">
+        <v>115</v>
+      </c>
+      <c r="N177" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>90</v>
       </c>
@@ -11747,12 +11959,48 @@
         <f>27665/3011</f>
         <v>9.1879774161408179</v>
       </c>
+      <c r="C178">
+        <f>28349/3149</f>
+        <v>9.0025404890441418</v>
+      </c>
+      <c r="D178">
+        <f>27874/3054</f>
+        <v>9.127046496398167</v>
+      </c>
+      <c r="E178">
+        <f>30408/3093</f>
+        <v>9.8312318137730355</v>
+      </c>
+      <c r="F178">
+        <f>30552/3154</f>
+        <v>9.6867469879518069</v>
+      </c>
+      <c r="H178">
+        <f>27287/3026</f>
+        <v>9.0175148711169868</v>
+      </c>
+      <c r="I178">
+        <f>29005/3012</f>
+        <v>9.6298140770252321</v>
+      </c>
       <c r="J178">
         <f>20337/2000</f>
         <v>10.1685</v>
       </c>
-    </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L178">
+        <f>AVERAGE(B178:J178)</f>
+        <v>9.4564215189312737</v>
+      </c>
+      <c r="M178">
+        <f>AVERAGE(B178:H178)</f>
+        <v>9.308843012404159</v>
+      </c>
+      <c r="N178">
+        <f>AVERAGE(I178:J178)</f>
+        <v>9.899157038512616</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>91</v>
       </c>
@@ -11760,12 +12008,48 @@
         <f>21977/3011</f>
         <v>7.2989040185984724</v>
       </c>
+      <c r="C179">
+        <f>23656/3149</f>
+        <v>7.5122261035249283</v>
+      </c>
+      <c r="D179">
+        <f>24225/3054</f>
+        <v>7.9322200392927309</v>
+      </c>
+      <c r="E179">
+        <f>26364/3093</f>
+        <v>8.5237633365664411</v>
+      </c>
+      <c r="F179">
+        <f>26706/3154</f>
+        <v>8.4673430564362722</v>
+      </c>
+      <c r="H179">
+        <f>24405/3026</f>
+        <v>8.0651024454725704</v>
+      </c>
+      <c r="I179">
+        <f>22464/3012</f>
+        <v>7.4581673306772904</v>
+      </c>
       <c r="J179">
         <f>15733/2000</f>
         <v>7.8665000000000003</v>
       </c>
-    </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L179">
+        <f>AVERAGE(B179:J179)</f>
+        <v>7.8905282913210879</v>
+      </c>
+      <c r="M179">
+        <f>AVERAGE(B179:H179)</f>
+        <v>7.9665931666485683</v>
+      </c>
+      <c r="N179">
+        <f t="shared" ref="N179:N180" si="7">AVERAGE(I179:J179)</f>
+        <v>7.6623336653386449</v>
+      </c>
+    </row>
+    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>92</v>
       </c>
@@ -11773,9 +12057,45 @@
         <f>830515/3011</f>
         <v>275.82696778478913</v>
       </c>
+      <c r="C180">
+        <f>836547/3149</f>
+        <v>265.65481105112735</v>
+      </c>
+      <c r="D180">
+        <f>844315/3054</f>
+        <v>276.46201702685005</v>
+      </c>
+      <c r="E180">
+        <f>800038/3093</f>
+        <v>258.66084707403814</v>
+      </c>
+      <c r="F180">
+        <f>968130/3154</f>
+        <v>306.95307545973367</v>
+      </c>
+      <c r="H180">
+        <f>1215430/3026</f>
+        <v>401.66226040978188</v>
+      </c>
+      <c r="I180">
+        <f>1061965/3012</f>
+        <v>352.57802124833995</v>
+      </c>
       <c r="J180">
         <f>600977/2000</f>
         <v>300.48849999999999</v>
+      </c>
+      <c r="L180">
+        <f>AVERAGE(B180:J180)</f>
+        <v>304.78581250683254</v>
+      </c>
+      <c r="M180">
+        <f>AVERAGE(B180:H180)</f>
+        <v>297.53666313438674</v>
+      </c>
+      <c r="N180">
+        <f t="shared" si="7"/>
+        <v>326.53326062417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>